<commit_message>
Monster CSV loading, monsters face left or right.  Code cleanup.
</commit_message>
<xml_diff>
--- a/Maps/map_workbook.xlsx
+++ b/Maps/map_workbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markpontius/Desktop/Programming/C/Dungeon-Reincarnate-1/Maps/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markpontius/Desktop/Programming/C/XCode/Dungeon Reincarnate XCode/Dungeon Reincarnate/Maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AD358E80-82D2-564F-81C7-5000F0495823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00C5C03-1E31-B742-866E-2BCDCFCE87F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6360" yWindow="6420" windowWidth="20300" windowHeight="10380" firstSheet="1" activeTab="9" xr2:uid="{BFB22DB9-C1C3-2D48-9E01-F98DEC5CE4B6}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3186" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3193" uniqueCount="443">
   <si>
     <t>dir</t>
   </si>
@@ -1235,9 +1235,6 @@
     <t>209D</t>
   </si>
   <si>
-    <t>uid</t>
-  </si>
-  <si>
     <t>common_type</t>
   </si>
   <si>
@@ -1256,9 +1253,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>map_num</t>
-  </si>
-  <si>
     <t>speed</t>
   </si>
   <si>
@@ -1274,15 +1268,6 @@
     <t>AC</t>
   </si>
   <si>
-    <t>option_graphic_dir</t>
-  </si>
-  <si>
-    <t>option_open_doors</t>
-  </si>
-  <si>
-    <t>option_close_doors</t>
-  </si>
-  <si>
     <t>Mimic</t>
   </si>
   <si>
@@ -1352,9 +1337,6 @@
     <t>A spritely orange ghost</t>
   </si>
   <si>
-    <t>A spritely pruple ghoat</t>
-  </si>
-  <si>
     <t>mode</t>
   </si>
   <si>
@@ -1362,6 +1344,39 @@
   </si>
   <si>
     <t>A53AFFFF</t>
+  </si>
+  <si>
+    <t>#uid</t>
+  </si>
+  <si>
+    <t>A spritely pruple ghost</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>A fearsome fire breathing dragon</t>
+  </si>
+  <si>
+    <t>D4AF37</t>
+  </si>
+  <si>
+    <t>Claw</t>
+  </si>
+  <si>
+    <t>graphic_dir</t>
+  </si>
+  <si>
+    <t>open_doors</t>
+  </si>
+  <si>
+    <t>close_doors</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>PNG/dragon-ultima3-white.png</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1556,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -5244,148 +5259,148 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0017427-9753-2942-A63B-454AF996185A}">
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="5.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6" style="12" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" style="12" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="24" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
+        <v>432</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>399</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>441</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>395</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="17" t="s">
+      <c r="H1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>429</v>
+      </c>
+      <c r="K1" s="17" t="s">
         <v>396</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>435</v>
-      </c>
-      <c r="G1" s="17" t="s">
+      <c r="L1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="N1" s="17" t="s">
         <v>397</v>
       </c>
-      <c r="H1" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="J1" s="17" t="s">
+      <c r="O1" s="17" t="s">
         <v>398</v>
       </c>
-      <c r="K1" s="17" t="s">
-        <v>399</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>400</v>
-      </c>
-      <c r="M1" s="17" t="s">
+      <c r="P1" s="17" t="s">
         <v>401</v>
       </c>
-      <c r="N1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="17" t="s">
+      <c r="Q1" s="17" t="s">
         <v>402</v>
       </c>
-      <c r="P1" s="17" t="s">
+      <c r="R1" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="S1" s="17" t="s">
         <v>404</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="T1" s="17" t="s">
         <v>405</v>
       </c>
-      <c r="S1" s="17" t="s">
-        <v>406</v>
-      </c>
-      <c r="T1" s="17" t="s">
-        <v>407</v>
-      </c>
       <c r="U1" s="17" t="s">
-        <v>408</v>
+        <v>438</v>
       </c>
       <c r="V1" s="17" t="s">
-        <v>409</v>
+        <v>439</v>
       </c>
       <c r="W1" s="17" t="s">
-        <v>410</v>
+        <v>440</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>411</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" s="12">
+        <v>10.5</v>
+      </c>
+      <c r="C2" s="12">
+        <v>10.5</v>
+      </c>
+      <c r="D2" s="12">
+        <v>3</v>
+      </c>
+      <c r="E2" s="12">
+        <v>1</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>412</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>413</v>
-      </c>
-      <c r="F2" s="12">
+      <c r="H2" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="J2" s="12">
         <v>2</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>414</v>
-      </c>
-      <c r="H2" s="12">
+      <c r="K2" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="L2" s="12">
         <v>0.75</v>
       </c>
-      <c r="I2" s="12">
-        <v>1</v>
-      </c>
-      <c r="L2" s="12">
-        <v>10.5</v>
-      </c>
       <c r="M2" s="12">
-        <v>10.5</v>
-      </c>
-      <c r="N2" s="12">
-        <v>3</v>
-      </c>
-      <c r="O2" s="12">
         <v>1</v>
       </c>
       <c r="P2" s="12">
@@ -5398,7 +5413,7 @@
         <v>2</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="T2" s="12">
         <v>8</v>
@@ -5417,44 +5432,44 @@
       <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>432</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>416</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="B3" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="C3" s="12">
+        <v>13.5</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="12">
+        <v>3</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>421</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="J3" s="12">
         <v>2</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>350</v>
       </c>
-      <c r="H3" s="12">
+      <c r="L3" s="12">
         <v>0.75</v>
       </c>
-      <c r="I3" s="12">
-        <v>1</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>427</v>
-      </c>
-      <c r="L3" s="12">
-        <v>1.5</v>
-      </c>
       <c r="M3" s="12">
-        <v>13.5</v>
-      </c>
-      <c r="N3" s="12">
-        <v>1</v>
-      </c>
-      <c r="O3" s="12">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>422</v>
       </c>
       <c r="P3" s="12">
         <v>0.05</v>
@@ -5466,7 +5481,7 @@
         <v>1</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="T3" s="12">
         <v>6</v>
@@ -5485,44 +5500,44 @@
       <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>418</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>421</v>
-      </c>
-      <c r="E4" s="12" t="s">
+      <c r="B4" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="C4" s="12">
+        <v>13.5</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>416</v>
       </c>
-      <c r="F4" s="12">
+      <c r="I4" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="J4" s="12">
         <v>2</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>417</v>
-      </c>
-      <c r="H4" s="12">
+      <c r="K4" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="L4" s="12">
         <v>0.75</v>
       </c>
-      <c r="I4" s="12">
-        <v>1</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="L4" s="12">
-        <v>1.5</v>
-      </c>
       <c r="M4" s="12">
-        <v>13.5</v>
-      </c>
-      <c r="N4" s="12">
-        <v>1</v>
-      </c>
-      <c r="O4" s="12">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>423</v>
       </c>
       <c r="P4" s="12">
         <v>0.05</v>
@@ -5534,7 +5549,7 @@
         <v>1</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="T4" s="12">
         <v>6</v>
@@ -5553,44 +5568,44 @@
       <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>423</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>422</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>416</v>
-      </c>
-      <c r="F5" s="12">
+      <c r="B5" s="12">
+        <v>11.5</v>
+      </c>
+      <c r="C5" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="D5" s="12">
+        <v>3</v>
+      </c>
+      <c r="E5" s="12">
+        <v>3</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="J5" s="12">
         <v>2</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>436</v>
-      </c>
-      <c r="H5" s="12">
+      <c r="K5" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="L5" s="12">
         <v>0.75</v>
       </c>
-      <c r="I5" s="12">
-        <v>1</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>429</v>
-      </c>
-      <c r="L5" s="12">
-        <v>11.5</v>
-      </c>
       <c r="M5" s="12">
-        <v>3.5</v>
-      </c>
-      <c r="N5" s="12">
-        <v>3</v>
-      </c>
-      <c r="O5" s="12">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>424</v>
       </c>
       <c r="P5" s="12">
         <v>0.05</v>
@@ -5602,7 +5617,7 @@
         <v>1</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="T5" s="12">
         <v>6</v>
@@ -5621,44 +5636,44 @@
       <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>433</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>416</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="B6" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="C6" s="12">
+        <v>13.5</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12">
+        <v>3</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="J6" s="12">
         <v>2</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>417</v>
-      </c>
-      <c r="H6" s="12">
+      <c r="K6" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="L6" s="12">
         <v>0.75</v>
       </c>
-      <c r="I6" s="12">
-        <v>1</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>430</v>
-      </c>
-      <c r="L6" s="12">
-        <v>1.5</v>
-      </c>
       <c r="M6" s="12">
-        <v>13.5</v>
-      </c>
-      <c r="N6" s="12">
-        <v>1</v>
-      </c>
-      <c r="O6" s="12">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>425</v>
       </c>
       <c r="P6" s="12">
         <v>0.05</v>
@@ -5670,7 +5685,7 @@
         <v>1</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="T6" s="12">
         <v>6</v>
@@ -5689,44 +5704,44 @@
       <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>425</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>434</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>416</v>
-      </c>
-      <c r="F7" s="12">
+      <c r="B7" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="C7" s="12">
+        <v>13.5</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1</v>
+      </c>
+      <c r="E7" s="12">
+        <v>3</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>433</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="J7" s="12">
         <v>2</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>437</v>
-      </c>
-      <c r="H7" s="12">
+      <c r="K7" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="L7" s="12">
         <v>0.75</v>
       </c>
-      <c r="I7" s="12">
-        <v>1</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>431</v>
-      </c>
-      <c r="L7" s="12">
-        <v>1.5</v>
-      </c>
       <c r="M7" s="12">
-        <v>13.5</v>
-      </c>
-      <c r="N7" s="12">
-        <v>1</v>
-      </c>
-      <c r="O7" s="12">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>426</v>
       </c>
       <c r="P7" s="12">
         <v>0.05</v>
@@ -5738,7 +5753,7 @@
         <v>1</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="T7" s="12">
         <v>6</v>
@@ -5750,6 +5765,74 @@
         <v>0</v>
       </c>
       <c r="W7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>32.5</v>
+      </c>
+      <c r="C8" s="12">
+        <v>32.5</v>
+      </c>
+      <c r="D8" s="12">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12">
+        <v>4</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="J8" s="12">
+        <v>2</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="L8" s="12">
+        <v>1</v>
+      </c>
+      <c r="M8" s="12">
+        <v>1</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>20</v>
+      </c>
+      <c r="R8" s="12">
+        <v>4</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="T8" s="12">
+        <v>4</v>
+      </c>
+      <c r="U8" s="12">
+        <v>0</v>
+      </c>
+      <c r="V8" s="12">
+        <v>0</v>
+      </c>
+      <c r="W8" s="12">
         <v>0</v>
       </c>
     </row>

</xml_diff>